<commit_message>
Test Cases Updated and Logger Updated.
</commit_message>
<xml_diff>
--- a/appseConnectV1/src/test/java/com/appseConnect/testData/LoginData.xlsx
+++ b/appseConnectV1/src/test/java/com/appseConnect/testData/LoginData.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{643202C6-C541-4FB5-AC71-C9026F36B78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debashree\git\MyProductFrameworkSeleniumRepo\appseConnectV1\src\test\java\com\appseConnect\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF5CF5B-0288-4564-9402-114455EE49FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="19460" windowHeight="11060" xr2:uid="{93A7355B-BA15-4717-8935-5C3B7C926339}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93A7355B-BA15-4717-8935-5C3B7C926339}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>USERNAME</t>
   </si>
@@ -438,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0494A47-BF7E-4858-A2F3-A53AEA499EF6}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,11 +495,27 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -504,9 +524,10 @@
     <hyperlink ref="A3" r:id="rId2" xr:uid="{81C2FA38-6DB8-4B8E-99A9-61A190BB7E91}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{42F47189-9F49-4609-9C7E-9650702E7E66}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{BA895370-251E-44AC-A107-608FC67ECEFD}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{E0EE2E64-416C-4FCD-87EC-A24F1A74602E}"/>
+    <hyperlink ref="A7" r:id="rId5" xr:uid="{E0EE2E64-416C-4FCD-87EC-A24F1A74602E}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{D576C564-676B-4DFD-BDD5-C9F84D4975C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Cases added and updated
</commit_message>
<xml_diff>
--- a/appseConnectV1/src/test/java/com/appseConnect/testData/LoginData.xlsx
+++ b/appseConnectV1/src/test/java/com/appseConnect/testData/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debashree\git\MyProductFrameworkSeleniumRepo\appseConnectV1\src\test\java\com\appseConnect\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF5CF5B-0288-4564-9402-114455EE49FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC33990-EEAD-43BE-B711-B244B404CED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{93A7355B-BA15-4717-8935-5C3B7C926339}"/>
   </bookViews>
@@ -39,13 +39,13 @@
     <t>Efgh.1234</t>
   </si>
   <si>
+    <t>abcd.1234</t>
+  </si>
+  <si>
+    <t>rio1@yopmail.com</t>
+  </si>
+  <si>
     <t>Efgh.1234xxxx</t>
-  </si>
-  <si>
-    <t>rio1@yopmail.com</t>
-  </si>
-  <si>
-    <t>abcd.1234</t>
   </si>
   <si>
     <t>debashree.p@insync.co.inxxxxxxx</t>
@@ -445,7 +445,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,7 +475,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -495,37 +495,37 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B9398A00-D106-45D3-AC02-19108BCC952C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{81C2FA38-6DB8-4B8E-99A9-61A190BB7E91}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{42F47189-9F49-4609-9C7E-9650702E7E66}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{BA895370-251E-44AC-A107-608FC67ECEFD}"/>
-    <hyperlink ref="A7" r:id="rId5" xr:uid="{E0EE2E64-416C-4FCD-87EC-A24F1A74602E}"/>
-    <hyperlink ref="A8" r:id="rId6" xr:uid="{D576C564-676B-4DFD-BDD5-C9F84D4975C5}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{17E7C1CD-D415-41AF-B4CB-3A0A151B2455}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{85986FC0-7A34-488F-BA9D-10102E3A4CD9}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{081D4998-4B89-4098-8406-1AF4CF4BE9B1}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{B36FC40F-A846-47C3-A9D9-DA5D7C9D7447}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{E8C41D2B-9F87-4112-9965-4890ED37A099}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>